<commit_message>
oil time series 1
</commit_message>
<xml_diff>
--- a/Part3-ClusteringandModels/Prediction/PredictionResults.xlsx
+++ b/Part3-ClusteringandModels/Prediction/PredictionResults.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9140" yWindow="460" windowWidth="25380" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="9320" yWindow="460" windowWidth="22300" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,20 +80,20 @@
     <t>Neural Network</t>
   </si>
   <si>
-    <t>Improving Best Model</t>
-  </si>
-  <si>
     <t>Classes</t>
   </si>
   <si>
     <t>Azure RMSE</t>
+  </si>
+  <si>
+    <t>Feature Selection</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -102,8 +102,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -149,6 +150,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Menlo"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -172,23 +178,23 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -471,8 +477,8 @@
   <dimension ref="A1:L102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L93" sqref="L93"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G21" sqref="G21:J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -481,6 +487,7 @@
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="11"/>
     <col min="6" max="6" width="3.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
@@ -496,7 +503,7 @@
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2">
+      <c r="E1" s="8">
         <v>45628065</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -520,9 +527,9 @@
         <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -544,7 +551,7 @@
         <v>12</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.25">
@@ -557,25 +564,25 @@
       <c r="C3" s="2">
         <v>500000</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="4">
         <v>16</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="5">
         <v>1.0904594321100001</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="5">
         <v>1.0900729547500001</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="5">
         <v>60.472444308999997</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="5">
         <v>60.522581109599997</v>
       </c>
       <c r="K3" s="1"/>
@@ -586,20 +593,20 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="4"/>
+      <c r="E4" s="7"/>
       <c r="F4" s="1">
         <v>2</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="5">
         <v>1.08928277246</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="5">
         <v>1.0902197334499999</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="5">
         <v>60.436552897799999</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="5">
         <v>60.419177671999996</v>
       </c>
       <c r="K4" s="1"/>
@@ -610,22 +617,22 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="1">
         <v>1</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="5">
         <v>0.58650908511199995</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="5">
         <v>1.1728273253799999</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="5">
         <v>31.684440790699998</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="5">
         <v>64.3759440324</v>
       </c>
       <c r="K5" s="1"/>
@@ -636,20 +643,20 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="4"/>
+      <c r="E6" s="7"/>
       <c r="F6" s="1">
         <v>2</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="5">
         <v>0.58613668544399999</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="5">
         <v>1.17318312479</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="5">
         <v>31.683351230700001</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="5">
         <v>64.332423529699994</v>
       </c>
       <c r="K6" s="1"/>
@@ -660,22 +667,22 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="10" t="s">
         <v>15</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="5">
         <v>1.0930364835899999</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="5">
         <v>1.0940481903499999</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="5">
         <v>60.659718789499998</v>
       </c>
-      <c r="J7" s="8">
+      <c r="J7" s="5">
         <v>60.787817564299999</v>
       </c>
       <c r="K7" s="1"/>
@@ -686,20 +693,20 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="5"/>
+      <c r="E8" s="10"/>
       <c r="F8" s="1">
         <v>2</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="5">
         <v>1.0920670073600001</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="5">
         <v>1.09377428158</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="5">
         <v>60.634107444400001</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J8" s="5">
         <v>60.658074690600003</v>
       </c>
       <c r="K8" s="1"/>
@@ -716,16 +723,16 @@
       <c r="F9" s="1">
         <v>1</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="5">
         <v>1.0669544841800001</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="5">
         <v>1.08480978783</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="5">
         <v>58.662994638100002</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J9" s="5">
         <v>59.7490761679</v>
       </c>
       <c r="K9" s="1"/>
@@ -740,16 +747,16 @@
       <c r="F10" s="1">
         <v>2</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="5">
         <v>1.0520742133200001</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="5">
         <v>1.07357050058</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10" s="5">
         <v>56.792434765300001</v>
       </c>
-      <c r="J10" s="8">
+      <c r="J10" s="5">
         <v>57.931308583099998</v>
       </c>
       <c r="K10" s="1"/>
@@ -760,16 +767,16 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="4" t="s">
-        <v>17</v>
+      <c r="E11" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="F11" s="1">
         <v>1</v>
       </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
@@ -778,14 +785,14 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="4"/>
+      <c r="E12" s="7"/>
       <c r="F12" s="1">
         <v>2</v>
       </c>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
@@ -802,22 +809,22 @@
       <c r="D13" s="2">
         <v>9</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="5">
         <v>2.0993703402600001</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="5">
         <v>2.1046738778999998</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="5">
         <v>87.829126326500003</v>
       </c>
-      <c r="J13" s="8">
+      <c r="J13" s="5">
         <v>87.836176068599997</v>
       </c>
       <c r="K13" s="1"/>
@@ -828,20 +835,20 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="4"/>
+      <c r="E14" s="7"/>
       <c r="F14" s="1">
         <v>2</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="5">
         <v>2.1051507906800002</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="5">
         <v>2.1007661406799998</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="5">
         <v>87.889232182699999</v>
       </c>
-      <c r="J14" s="8">
+      <c r="J14" s="5">
         <v>87.924111797400002</v>
       </c>
       <c r="K14" s="1"/>
@@ -852,22 +859,22 @@
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F15" s="1">
         <v>1</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="5">
         <v>1.08728986683</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="5">
         <v>2.2546991569100001</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I15" s="5">
         <v>43.164961937900003</v>
       </c>
-      <c r="J15" s="8">
+      <c r="J15" s="5">
         <v>90.809824834699995</v>
       </c>
       <c r="K15" s="1"/>
@@ -878,20 +885,20 @@
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="4"/>
+      <c r="E16" s="7"/>
       <c r="F16" s="1">
         <v>2</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="5">
         <v>1.0884393397600001</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="5">
         <v>2.2522520039499998</v>
       </c>
-      <c r="I16" s="8">
+      <c r="I16" s="5">
         <v>43.152323474200003</v>
       </c>
-      <c r="J16" s="8">
+      <c r="J16" s="5">
         <v>90.9273331558</v>
       </c>
       <c r="K16" s="1"/>
@@ -902,22 +909,22 @@
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="10" t="s">
         <v>15</v>
       </c>
       <c r="F17" s="1">
         <v>1</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="5">
         <v>2.09206164729</v>
       </c>
-      <c r="H17" s="8">
+      <c r="H17" s="5">
         <v>2.09842649467</v>
       </c>
-      <c r="I17" s="9">
+      <c r="I17" s="6">
         <v>87.572149580499996</v>
       </c>
-      <c r="J17" s="8">
+      <c r="J17" s="5">
         <v>87.602485361399999</v>
       </c>
       <c r="K17" s="1"/>
@@ -928,20 +935,20 @@
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="5"/>
+      <c r="E18" s="10"/>
       <c r="F18" s="1">
         <v>2</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="5">
         <v>2.0961302366200001</v>
       </c>
-      <c r="H18" s="8">
+      <c r="H18" s="5">
         <v>2.0957629258999999</v>
       </c>
-      <c r="I18" s="8">
+      <c r="I18" s="5">
         <v>87.460341781799997</v>
       </c>
-      <c r="J18" s="8">
+      <c r="J18" s="5">
         <v>87.667197371300006</v>
       </c>
       <c r="K18" s="1"/>
@@ -958,16 +965,16 @@
       <c r="F19" s="1">
         <v>1</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="5">
         <v>2.00740420695</v>
       </c>
-      <c r="H19" s="8">
+      <c r="H19" s="5">
         <v>2.0486595379299999</v>
       </c>
-      <c r="I19" s="8">
+      <c r="I19" s="5">
         <v>79.325188486900004</v>
       </c>
-      <c r="J19" s="8">
+      <c r="J19" s="5">
         <v>80.854163675899997</v>
       </c>
       <c r="K19" s="1"/>
@@ -982,52 +989,68 @@
       <c r="F20" s="1">
         <v>2</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="5">
         <v>2.0357584218799998</v>
       </c>
-      <c r="H20" s="8">
+      <c r="H20" s="5">
         <v>2.07178149231</v>
       </c>
-      <c r="I20" s="8">
+      <c r="I20" s="5">
         <v>83.414331403099993</v>
       </c>
-      <c r="J20" s="8">
+      <c r="J20" s="5">
         <v>85.096921206199994</v>
       </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="4" t="s">
-        <v>17</v>
+      <c r="E21" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="F21" s="1">
         <v>1</v>
       </c>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
+      <c r="G21" s="5">
+        <v>2.1025469075899998</v>
+      </c>
+      <c r="H21" s="5">
+        <v>2.1030154164799999</v>
+      </c>
+      <c r="I21" s="5">
+        <v>87.791265508699993</v>
+      </c>
+      <c r="J21" s="5">
+        <v>88.103833214299996</v>
+      </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="17" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="4"/>
+      <c r="E22" s="7"/>
       <c r="F22" s="1">
         <v>2</v>
       </c>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
+      <c r="G22" s="5">
+        <v>2.1020486280799999</v>
+      </c>
+      <c r="H22" s="5">
+        <v>2.1022706920099998</v>
+      </c>
+      <c r="I22" s="5">
+        <v>87.9317726214</v>
+      </c>
+      <c r="J22" s="5">
+        <v>87.652838326700007</v>
+      </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
     </row>
@@ -1044,46 +1067,50 @@
       <c r="D23" s="2">
         <v>1</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F23" s="1">
         <v>1</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="5">
         <v>4.9462765615200004</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="5">
         <v>5.0075030832599996</v>
       </c>
-      <c r="I23" s="8">
+      <c r="I23" s="5">
         <v>115.838648041</v>
       </c>
-      <c r="J23" s="8">
+      <c r="J23" s="5">
         <v>117.783078074</v>
       </c>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
+      <c r="K23">
+        <v>4.9862229999999998</v>
+      </c>
+      <c r="L23">
+        <v>6.2794210000000001</v>
+      </c>
     </row>
     <row r="24" spans="1:12" ht="17" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="4"/>
+      <c r="E24" s="7"/>
       <c r="F24" s="1">
         <v>2</v>
       </c>
-      <c r="G24" s="8">
+      <c r="G24" s="5">
         <v>5.01142071704</v>
       </c>
-      <c r="H24" s="8">
+      <c r="H24" s="5">
         <v>4.9588547289099996</v>
       </c>
-      <c r="I24" s="8">
+      <c r="I24" s="5">
         <v>118.009440807</v>
       </c>
-      <c r="J24" s="8">
+      <c r="J24" s="5">
         <v>116.32570312</v>
       </c>
       <c r="K24" s="1"/>
@@ -1094,22 +1121,22 @@
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F25" s="1">
         <v>1</v>
       </c>
-      <c r="G25" s="8">
+      <c r="G25" s="5">
         <v>2.4709465492199998</v>
       </c>
-      <c r="H25" s="8">
+      <c r="H25" s="5">
         <v>5.3284163633499997</v>
       </c>
-      <c r="I25" s="8">
+      <c r="I25" s="5">
         <v>53.7062162203</v>
       </c>
-      <c r="J25" s="8">
+      <c r="J25" s="5">
         <v>118.850403715</v>
       </c>
       <c r="K25" s="1"/>
@@ -1120,20 +1147,20 @@
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
-      <c r="E26" s="4"/>
+      <c r="E26" s="7"/>
       <c r="F26" s="1">
         <v>2</v>
       </c>
-      <c r="G26" s="8">
+      <c r="G26" s="5">
         <v>2.5046458651100001</v>
       </c>
-      <c r="H26" s="8">
+      <c r="H26" s="5">
         <v>5.3154359875099999</v>
       </c>
-      <c r="I26" s="8">
+      <c r="I26" s="5">
         <v>55.046736234500003</v>
       </c>
-      <c r="J26" s="8">
+      <c r="J26" s="5">
         <v>118.36590058100001</v>
       </c>
       <c r="K26" s="1"/>
@@ -1144,22 +1171,22 @@
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="5" t="s">
+      <c r="E27" s="10" t="s">
         <v>15</v>
       </c>
       <c r="F27" s="1">
         <v>1</v>
       </c>
-      <c r="G27" s="8">
+      <c r="G27" s="5">
         <v>4.9282818774399999</v>
       </c>
-      <c r="H27" s="8">
+      <c r="H27" s="5">
         <v>4.9966493162600001</v>
       </c>
-      <c r="I27" s="8">
+      <c r="I27" s="5">
         <v>115.57292504999999</v>
       </c>
-      <c r="J27" s="8">
+      <c r="J27" s="5">
         <v>117.408977858</v>
       </c>
       <c r="K27" s="1"/>
@@ -1170,20 +1197,20 @@
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
-      <c r="E28" s="5"/>
+      <c r="E28" s="10"/>
       <c r="F28" s="1">
         <v>2</v>
       </c>
-      <c r="G28" s="8">
+      <c r="G28" s="5">
         <v>4.9943057961399999</v>
       </c>
-      <c r="H28" s="8">
+      <c r="H28" s="5">
         <v>4.9570607209800004</v>
       </c>
-      <c r="I28" s="8">
+      <c r="I28" s="5">
         <v>117.854739017</v>
       </c>
-      <c r="J28" s="8">
+      <c r="J28" s="5">
         <v>116.771701806</v>
       </c>
       <c r="K28" s="1"/>
@@ -1200,16 +1227,16 @@
       <c r="F29" s="1">
         <v>1</v>
       </c>
-      <c r="G29" s="8">
+      <c r="G29" s="5">
         <v>4.7511376520299997</v>
       </c>
-      <c r="H29" s="8">
+      <c r="H29" s="5">
         <v>5.0173551290200002</v>
       </c>
-      <c r="I29" s="8">
+      <c r="I29" s="5">
         <v>109.803531652</v>
       </c>
-      <c r="J29" s="8">
+      <c r="J29" s="5">
         <v>116.695205984</v>
       </c>
       <c r="K29" s="1"/>
@@ -1224,52 +1251,68 @@
       <c r="F30" s="1">
         <v>2</v>
       </c>
-      <c r="G30" s="8">
+      <c r="G30" s="5">
         <v>4.79822786062</v>
       </c>
-      <c r="H30" s="8">
+      <c r="H30" s="5">
         <v>4.9756339858400001</v>
       </c>
-      <c r="I30" s="8">
+      <c r="I30" s="5">
         <v>112.670762756</v>
       </c>
-      <c r="J30" s="8">
+      <c r="J30" s="5">
         <v>116.60307369500001</v>
       </c>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
     </row>
-    <row r="31" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
-      <c r="E31" s="4" t="s">
-        <v>17</v>
+      <c r="E31" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="F31" s="1">
         <v>1</v>
       </c>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
+      <c r="G31" s="5">
+        <v>4.9653838957799996</v>
+      </c>
+      <c r="H31" s="5">
+        <v>4.9933612650499999</v>
+      </c>
+      <c r="I31" s="5">
+        <v>116.37861061300001</v>
+      </c>
+      <c r="J31" s="5">
+        <v>117.131367197</v>
+      </c>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="17" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
-      <c r="E32" s="4"/>
+      <c r="E32" s="7"/>
       <c r="F32" s="1">
         <v>2</v>
       </c>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
+      <c r="G32" s="5">
+        <v>4.9933453596900002</v>
+      </c>
+      <c r="H32" s="5">
+        <v>4.9725560749</v>
+      </c>
+      <c r="I32" s="5">
+        <v>117.506191046</v>
+      </c>
+      <c r="J32" s="5">
+        <v>116.950252918</v>
+      </c>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
     </row>
@@ -1292,20 +1335,24 @@
       <c r="F33" s="1">
         <v>1</v>
       </c>
-      <c r="G33" s="8">
+      <c r="G33" s="5">
         <v>3.6987785745299999</v>
       </c>
-      <c r="H33" s="8">
+      <c r="H33" s="5">
         <v>3.6956420527299998</v>
       </c>
-      <c r="I33" s="8">
+      <c r="I33" s="5">
         <v>118.355929414</v>
       </c>
-      <c r="J33" s="8">
+      <c r="J33" s="5">
         <v>118.107319756</v>
       </c>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
+      <c r="K33">
+        <v>3.6975090000000002</v>
+      </c>
+      <c r="L33">
+        <v>4.7645400000000002</v>
+      </c>
     </row>
     <row r="34" spans="1:12" ht="17" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
@@ -1316,16 +1363,16 @@
       <c r="F34" s="1">
         <v>2</v>
       </c>
-      <c r="G34" s="8">
+      <c r="G34" s="5">
         <v>3.69377823031</v>
       </c>
-      <c r="H34" s="8">
+      <c r="H34" s="5">
         <v>3.6993573669000002</v>
       </c>
-      <c r="I34" s="8">
+      <c r="I34" s="5">
         <v>118.03784750299999</v>
       </c>
-      <c r="J34" s="8">
+      <c r="J34" s="5">
         <v>118.388289814</v>
       </c>
       <c r="K34" s="1"/>
@@ -1336,22 +1383,22 @@
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="4" t="s">
+      <c r="E35" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F35" s="1">
         <v>1</v>
       </c>
-      <c r="G35" s="8">
+      <c r="G35" s="5">
         <v>2.3971780768099999</v>
       </c>
-      <c r="H35" s="8">
+      <c r="H35" s="5">
         <v>4.1750034035099999</v>
       </c>
-      <c r="I35" s="8">
+      <c r="I35" s="5">
         <v>70.412964053799996</v>
       </c>
-      <c r="J35" s="8">
+      <c r="J35" s="5">
         <v>124.592471277</v>
       </c>
       <c r="K35" s="1"/>
@@ -1362,20 +1409,20 @@
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
-      <c r="E36" s="4"/>
+      <c r="E36" s="7"/>
       <c r="F36" s="1">
         <v>2</v>
       </c>
-      <c r="G36" s="8">
+      <c r="G36" s="5">
         <v>2.3989830969699999</v>
       </c>
-      <c r="H36" s="8">
+      <c r="H36" s="5">
         <v>4.1745923855899996</v>
       </c>
-      <c r="I36" s="8">
+      <c r="I36" s="5">
         <v>70.3133271393</v>
       </c>
-      <c r="J36" s="8">
+      <c r="J36" s="5">
         <v>125.2354524</v>
       </c>
       <c r="K36" s="1"/>
@@ -1386,22 +1433,22 @@
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
-      <c r="E37" s="5" t="s">
+      <c r="E37" s="10" t="s">
         <v>15</v>
       </c>
       <c r="F37" s="1">
         <v>1</v>
       </c>
-      <c r="G37" s="8">
+      <c r="G37" s="5">
         <v>3.6947856180500001</v>
       </c>
-      <c r="H37" s="8">
+      <c r="H37" s="5">
         <v>3.7025079226200002</v>
       </c>
-      <c r="I37" s="8">
+      <c r="I37" s="5">
         <v>118.955741999</v>
       </c>
-      <c r="J37" s="8">
+      <c r="J37" s="5">
         <v>118.89816594200001</v>
       </c>
       <c r="K37" s="1"/>
@@ -1412,20 +1459,20 @@
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
-      <c r="E38" s="5"/>
+      <c r="E38" s="10"/>
       <c r="F38" s="1">
         <v>2</v>
       </c>
-      <c r="G38" s="8">
+      <c r="G38" s="5">
         <v>3.6938135909000001</v>
       </c>
-      <c r="H38" s="8">
+      <c r="H38" s="5">
         <v>3.7026930936900002</v>
       </c>
-      <c r="I38" s="8">
+      <c r="I38" s="5">
         <v>118.525019214</v>
       </c>
-      <c r="J38" s="8">
+      <c r="J38" s="5">
         <v>119.082422987</v>
       </c>
       <c r="K38" s="1"/>
@@ -1436,22 +1483,22 @@
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
-      <c r="E39" s="4" t="s">
+      <c r="E39" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F39" s="1">
         <v>1</v>
       </c>
-      <c r="G39" s="8">
+      <c r="G39" s="5">
         <v>4.9311429106000002</v>
       </c>
-      <c r="H39" s="8">
+      <c r="H39" s="5">
         <v>5.0300158052099997</v>
       </c>
-      <c r="I39" s="8">
+      <c r="I39" s="5">
         <v>129.722023831</v>
       </c>
-      <c r="J39" s="8">
+      <c r="J39" s="5">
         <v>131.833158508</v>
       </c>
       <c r="K39" s="1"/>
@@ -1462,56 +1509,72 @@
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
-      <c r="E40" s="4"/>
+      <c r="E40" s="7"/>
       <c r="F40" s="1">
         <v>2</v>
       </c>
-      <c r="G40" s="8">
+      <c r="G40" s="5">
         <v>4.86377244088</v>
       </c>
-      <c r="H40" s="8">
+      <c r="H40" s="5">
         <v>4.9527855971100001</v>
       </c>
-      <c r="I40" s="8">
+      <c r="I40" s="5">
         <v>125.038205439</v>
       </c>
-      <c r="J40" s="8">
+      <c r="J40" s="5">
         <v>127.79004286599999</v>
       </c>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
     </row>
-    <row r="41" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
-      <c r="E41" s="4" t="s">
-        <v>17</v>
+      <c r="E41" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="F41" s="1">
         <v>1</v>
       </c>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
+      <c r="G41" s="5">
+        <v>3.6988468891999999</v>
+      </c>
+      <c r="H41" s="5">
+        <v>3.69777795748</v>
+      </c>
+      <c r="I41" s="5">
+        <v>118.102237856</v>
+      </c>
+      <c r="J41" s="5">
+        <v>118.606646727</v>
+      </c>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" ht="17" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
-      <c r="E42" s="4"/>
+      <c r="E42" s="7"/>
       <c r="F42" s="1">
         <v>2</v>
       </c>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
+      <c r="G42" s="5">
+        <v>3.69341279574</v>
+      </c>
+      <c r="H42" s="5">
+        <v>3.6970235580800002</v>
+      </c>
+      <c r="I42" s="5">
+        <v>118.275451152</v>
+      </c>
+      <c r="J42" s="5">
+        <v>117.856044895</v>
+      </c>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
     </row>
@@ -1525,7 +1588,7 @@
       <c r="C43" s="2">
         <v>500000</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D43" s="4">
         <v>21</v>
       </c>
       <c r="E43" s="7" t="s">
@@ -1534,16 +1597,16 @@
       <c r="F43" s="1">
         <v>1</v>
       </c>
-      <c r="G43" s="8">
+      <c r="G43" s="5">
         <v>1.60452993812</v>
       </c>
-      <c r="H43" s="8">
+      <c r="H43" s="5">
         <v>1.60753634475</v>
       </c>
-      <c r="I43" s="8">
+      <c r="I43" s="5">
         <v>75.6795277545</v>
       </c>
-      <c r="J43" s="8">
+      <c r="J43" s="5">
         <v>75.833820897699994</v>
       </c>
       <c r="K43">
@@ -1562,16 +1625,16 @@
       <c r="F44" s="1">
         <v>2</v>
       </c>
-      <c r="G44" s="8">
+      <c r="G44" s="5">
         <v>1.60777786903</v>
       </c>
-      <c r="H44" s="8">
+      <c r="H44" s="5">
         <v>1.60563785684</v>
       </c>
-      <c r="I44" s="8">
+      <c r="I44" s="5">
         <v>75.833508001699997</v>
       </c>
-      <c r="J44" s="8">
+      <c r="J44" s="5">
         <v>75.722762407999994</v>
       </c>
       <c r="K44" s="1"/>
@@ -1582,22 +1645,22 @@
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
-      <c r="E45" s="4" t="s">
+      <c r="E45" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F45" s="1">
         <v>1</v>
       </c>
-      <c r="G45" s="8">
+      <c r="G45" s="5">
         <v>0.73874315712399996</v>
       </c>
-      <c r="H45" s="8">
+      <c r="H45" s="5">
         <v>1.70469996145</v>
       </c>
-      <c r="I45" s="8">
+      <c r="I45" s="5">
         <v>33.736290205099998</v>
       </c>
-      <c r="J45" s="8">
+      <c r="J45" s="5">
         <v>78.886062308800007</v>
       </c>
       <c r="K45" s="1"/>
@@ -1608,20 +1671,20 @@
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
-      <c r="E46" s="4"/>
+      <c r="E46" s="7"/>
       <c r="F46" s="1">
         <v>2</v>
       </c>
-      <c r="G46" s="9">
+      <c r="G46" s="6">
         <v>0.73914415180000004</v>
       </c>
-      <c r="H46" s="8">
+      <c r="H46" s="5">
         <v>1.70487898669</v>
       </c>
-      <c r="I46" s="8">
+      <c r="I46" s="5">
         <v>33.785295241699998</v>
       </c>
-      <c r="J46" s="8">
+      <c r="J46" s="5">
         <v>78.844605912700004</v>
       </c>
       <c r="K46" s="1"/>
@@ -1632,22 +1695,22 @@
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
-      <c r="E47" s="5" t="s">
+      <c r="E47" s="10" t="s">
         <v>15</v>
       </c>
       <c r="F47" s="1">
         <v>1</v>
       </c>
-      <c r="G47" s="8">
+      <c r="G47" s="5">
         <v>1.60229017465</v>
       </c>
-      <c r="H47" s="8">
+      <c r="H47" s="5">
         <v>1.6071516296199999</v>
       </c>
-      <c r="I47" s="8">
+      <c r="I47" s="5">
         <v>75.689052327599995</v>
       </c>
-      <c r="J47" s="8">
+      <c r="J47" s="5">
         <v>75.902904866399993</v>
       </c>
       <c r="K47" s="1"/>
@@ -1658,20 +1721,20 @@
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
-      <c r="E48" s="5"/>
+      <c r="E48" s="10"/>
       <c r="F48" s="1">
         <v>2</v>
       </c>
-      <c r="G48" s="8">
+      <c r="G48" s="5">
         <v>1.60567745642</v>
       </c>
-      <c r="H48" s="8">
+      <c r="H48" s="5">
         <v>1.6054439924299999</v>
       </c>
-      <c r="I48" s="8">
+      <c r="I48" s="5">
         <v>75.777146524100004</v>
       </c>
-      <c r="J48" s="8">
+      <c r="J48" s="5">
         <v>75.777200343299995</v>
       </c>
       <c r="K48" s="1"/>
@@ -1682,22 +1745,22 @@
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
-      <c r="E49" s="4" t="s">
+      <c r="E49" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F49" s="1">
         <v>1</v>
       </c>
-      <c r="G49" s="8">
+      <c r="G49" s="5">
         <v>1.59689036649</v>
       </c>
-      <c r="H49" s="8">
+      <c r="H49" s="5">
         <v>1.6390325560900001</v>
       </c>
-      <c r="I49" s="8">
+      <c r="I49" s="5">
         <v>76.666047988900004</v>
       </c>
-      <c r="J49" s="8">
+      <c r="J49" s="5">
         <v>78.689624527199996</v>
       </c>
       <c r="K49" s="1"/>
@@ -1708,20 +1771,20 @@
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
-      <c r="E50" s="4"/>
+      <c r="E50" s="7"/>
       <c r="F50" s="1">
         <v>2</v>
       </c>
-      <c r="G50" s="8">
+      <c r="G50" s="5">
         <v>1.57124687876</v>
       </c>
-      <c r="H50" s="8">
+      <c r="H50" s="5">
         <v>1.6088485100900001</v>
       </c>
-      <c r="I50" s="8">
+      <c r="I50" s="5">
         <v>73.356718263199994</v>
       </c>
-      <c r="J50" s="8">
+      <c r="J50" s="5">
         <v>75.165481913400001</v>
       </c>
       <c r="K50" s="1"/>
@@ -1732,22 +1795,22 @@
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
-      <c r="E51" s="4" t="s">
-        <v>17</v>
+      <c r="E51" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="F51" s="1">
         <v>1</v>
       </c>
-      <c r="G51" s="8">
+      <c r="G51" s="5">
         <v>1.6060007063799999</v>
       </c>
-      <c r="H51" s="8">
+      <c r="H51" s="5">
         <v>1.6063167270200001</v>
       </c>
-      <c r="I51" s="8">
+      <c r="I51" s="5">
         <v>75.749321275200003</v>
       </c>
-      <c r="J51" s="8">
+      <c r="J51" s="5">
         <v>75.817144131700005</v>
       </c>
       <c r="K51" s="1"/>
@@ -1758,20 +1821,20 @@
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
-      <c r="E52" s="4"/>
+      <c r="E52" s="7"/>
       <c r="F52" s="1">
         <v>2</v>
       </c>
-      <c r="G52" s="8">
+      <c r="G52" s="5">
         <v>1.6063114138600001</v>
       </c>
-      <c r="H52" s="8">
+      <c r="H52" s="5">
         <v>1.6065019522099999</v>
       </c>
-      <c r="I52" s="8">
+      <c r="I52" s="5">
         <v>75.770596614900001</v>
       </c>
-      <c r="J52" s="8">
+      <c r="J52" s="5">
         <v>75.725728650700006</v>
       </c>
       <c r="K52" s="1"/>
@@ -1796,16 +1859,16 @@
       <c r="F53" s="1">
         <v>1</v>
       </c>
-      <c r="G53" s="8">
+      <c r="G53" s="5">
         <v>0.52264630524900002</v>
       </c>
-      <c r="H53" s="8">
+      <c r="H53" s="5">
         <v>0.534347661827</v>
       </c>
-      <c r="I53" s="8">
+      <c r="I53" s="5">
         <v>36.955909245599997</v>
       </c>
-      <c r="J53" s="8">
+      <c r="J53" s="5">
         <v>37.363800187199999</v>
       </c>
       <c r="K53" s="1"/>
@@ -1820,16 +1883,16 @@
       <c r="F54" s="1">
         <v>2</v>
       </c>
-      <c r="G54" s="8">
+      <c r="G54" s="5">
         <v>0.53783846476399999</v>
       </c>
-      <c r="H54" s="8">
+      <c r="H54" s="5">
         <v>0.53562029967400004</v>
       </c>
-      <c r="I54" s="8">
+      <c r="I54" s="5">
         <v>38.052411659999997</v>
       </c>
-      <c r="J54" s="8">
+      <c r="J54" s="5">
         <v>38.339335697700001</v>
       </c>
       <c r="K54">
@@ -1844,22 +1907,22 @@
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
-      <c r="E55" s="4" t="s">
+      <c r="E55" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F55" s="1">
         <v>1</v>
       </c>
-      <c r="G55" s="8">
+      <c r="G55" s="5">
         <v>0.19588430283700001</v>
       </c>
-      <c r="H55" s="8">
+      <c r="H55" s="5">
         <v>0.53213859123100005</v>
       </c>
-      <c r="I55" s="8">
+      <c r="I55" s="5">
         <v>14.063364184699999</v>
       </c>
-      <c r="J55" s="8">
+      <c r="J55" s="5">
         <v>37.7087817476</v>
       </c>
       <c r="K55" s="1"/>
@@ -1870,20 +1933,20 @@
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
-      <c r="E56" s="4"/>
+      <c r="E56" s="7"/>
       <c r="F56" s="1">
         <v>2</v>
       </c>
-      <c r="G56" s="8">
+      <c r="G56" s="5">
         <v>0.20327995854399999</v>
       </c>
-      <c r="H56" s="8">
+      <c r="H56" s="5">
         <v>0.539006897589</v>
       </c>
-      <c r="I56" s="8">
+      <c r="I56" s="5">
         <v>14.6364186778</v>
       </c>
-      <c r="J56" s="8">
+      <c r="J56" s="5">
         <v>39.355409782999999</v>
       </c>
       <c r="K56" s="1"/>
@@ -1894,22 +1957,22 @@
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
-      <c r="E57" s="5" t="s">
+      <c r="E57" s="10" t="s">
         <v>15</v>
       </c>
       <c r="F57" s="1">
         <v>1</v>
       </c>
-      <c r="G57" s="8">
+      <c r="G57" s="5">
         <v>0.52924592750800004</v>
       </c>
-      <c r="H57" s="8">
+      <c r="H57" s="5">
         <v>0.53890939035600005</v>
       </c>
-      <c r="I57" s="8">
+      <c r="I57" s="5">
         <v>37.290040957400002</v>
       </c>
-      <c r="J57" s="8">
+      <c r="J57" s="5">
         <v>37.512458008300001</v>
       </c>
       <c r="K57" s="1"/>
@@ -1920,20 +1983,20 @@
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
-      <c r="E58" s="5"/>
+      <c r="E58" s="10"/>
       <c r="F58" s="1">
         <v>2</v>
       </c>
-      <c r="G58" s="8">
+      <c r="G58" s="5">
         <v>0.54137213177200005</v>
       </c>
-      <c r="H58" s="8">
+      <c r="H58" s="5">
         <v>0.54037275447699995</v>
       </c>
-      <c r="I58" s="8">
+      <c r="I58" s="5">
         <v>38.184260516999998</v>
       </c>
-      <c r="J58" s="8">
+      <c r="J58" s="5">
         <v>38.535442465499997</v>
       </c>
       <c r="K58" s="1"/>
@@ -1944,22 +2007,22 @@
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
-      <c r="E59" s="4" t="s">
+      <c r="E59" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F59" s="1">
         <v>1</v>
       </c>
-      <c r="G59" s="8">
+      <c r="G59" s="5">
         <v>0.35960472282900002</v>
       </c>
-      <c r="H59" s="8">
+      <c r="H59" s="5">
         <v>0.586569655799</v>
       </c>
-      <c r="I59" s="8">
+      <c r="I59" s="5">
         <v>25.785679484799999</v>
       </c>
-      <c r="J59" s="8">
+      <c r="J59" s="5">
         <v>41.88039886</v>
       </c>
       <c r="K59" s="1"/>
@@ -1970,20 +2033,20 @@
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
-      <c r="E60" s="4"/>
+      <c r="E60" s="7"/>
       <c r="F60" s="1">
         <v>2</v>
       </c>
-      <c r="G60" s="8">
+      <c r="G60" s="5">
         <v>0.40898519611700002</v>
       </c>
-      <c r="H60" s="8">
+      <c r="H60" s="5">
         <v>0.57757443515700002</v>
       </c>
-      <c r="I60" s="8">
+      <c r="I60" s="5">
         <v>29.7887270033</v>
       </c>
-      <c r="J60" s="9">
+      <c r="J60" s="6">
         <v>42.454508477200001</v>
       </c>
       <c r="K60" s="1"/>
@@ -1994,22 +2057,22 @@
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
-      <c r="E61" s="4" t="s">
-        <v>17</v>
+      <c r="E61" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="F61" s="1">
         <v>1</v>
       </c>
-      <c r="G61" s="8">
+      <c r="G61" s="5">
         <v>0.53862253197700005</v>
       </c>
-      <c r="H61" s="8">
+      <c r="H61" s="5">
         <v>0.53217206853200005</v>
       </c>
-      <c r="I61" s="8">
+      <c r="I61" s="5">
         <v>38.069474132499998</v>
       </c>
-      <c r="J61" s="8">
+      <c r="J61" s="5">
         <v>37.929548328300001</v>
       </c>
       <c r="K61" s="1"/>
@@ -2020,20 +2083,20 @@
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
-      <c r="E62" s="4"/>
+      <c r="E62" s="7"/>
       <c r="F62" s="1">
         <v>2</v>
       </c>
-      <c r="G62" s="8">
+      <c r="G62" s="5">
         <v>0.52622983699100001</v>
       </c>
-      <c r="H62" s="8">
+      <c r="H62" s="5">
         <v>0.53552723780099998</v>
       </c>
-      <c r="I62" s="8">
+      <c r="I62" s="5">
         <v>37.2447422718</v>
       </c>
-      <c r="J62" s="8">
+      <c r="J62" s="5">
         <v>37.532267793800003</v>
       </c>
       <c r="K62" s="1"/>
@@ -2058,16 +2121,16 @@
       <c r="F63" s="1">
         <v>1</v>
       </c>
-      <c r="G63" s="8">
+      <c r="G63" s="5">
         <v>2.6238135116999999</v>
       </c>
-      <c r="H63" s="8">
+      <c r="H63" s="5">
         <v>2.6136668297100001</v>
       </c>
-      <c r="I63" s="8">
+      <c r="I63" s="5">
         <v>99.1629727511</v>
       </c>
-      <c r="J63" s="8">
+      <c r="J63" s="5">
         <v>98.852082999900006</v>
       </c>
       <c r="K63">
@@ -2086,16 +2149,16 @@
       <c r="F64" s="1">
         <v>2</v>
       </c>
-      <c r="G64" s="8">
+      <c r="G64" s="5">
         <v>2.6130053845800001</v>
       </c>
-      <c r="H64" s="8">
+      <c r="H64" s="5">
         <v>2.6237913703300002</v>
       </c>
-      <c r="I64" s="8">
+      <c r="I64" s="5">
         <v>98.688494029500006</v>
       </c>
-      <c r="J64" s="9">
+      <c r="J64" s="6">
         <v>99.025397610499994</v>
       </c>
       <c r="K64" s="1"/>
@@ -2106,22 +2169,22 @@
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
-      <c r="E65" s="4" t="s">
+      <c r="E65" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F65" s="1">
         <v>1</v>
       </c>
-      <c r="G65" s="8">
+      <c r="G65" s="5">
         <v>1.5147338288800001</v>
       </c>
-      <c r="H65" s="8">
+      <c r="H65" s="5">
         <v>2.88523676887</v>
       </c>
-      <c r="I65" s="8">
+      <c r="I65" s="5">
         <v>53.5266282479</v>
       </c>
-      <c r="J65" s="8">
+      <c r="J65" s="5">
         <v>104.118826662</v>
       </c>
       <c r="K65" s="1"/>
@@ -2132,20 +2195,20 @@
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
-      <c r="E66" s="4"/>
+      <c r="E66" s="7"/>
       <c r="F66" s="1">
         <v>2</v>
       </c>
-      <c r="G66" s="8">
+      <c r="G66" s="5">
         <v>1.5087844375999999</v>
       </c>
-      <c r="H66" s="8">
+      <c r="H66" s="5">
         <v>2.8862424784099998</v>
       </c>
-      <c r="I66" s="8">
+      <c r="I66" s="5">
         <v>53.200607068499998</v>
       </c>
-      <c r="J66" s="8">
+      <c r="J66" s="5">
         <v>103.775197894</v>
       </c>
       <c r="K66" s="1"/>
@@ -2156,22 +2219,22 @@
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
-      <c r="E67" s="5" t="s">
+      <c r="E67" s="10" t="s">
         <v>15</v>
       </c>
       <c r="F67" s="1">
         <v>1</v>
       </c>
-      <c r="G67" s="8">
+      <c r="G67" s="5">
         <v>2.6199403766899998</v>
       </c>
-      <c r="H67" s="8">
+      <c r="H67" s="5">
         <v>2.6146808621300002</v>
       </c>
-      <c r="I67" s="8">
+      <c r="I67" s="5">
         <v>99.272126778699999</v>
       </c>
-      <c r="J67" s="8">
+      <c r="J67" s="5">
         <v>99.131956035599998</v>
       </c>
       <c r="K67" s="1"/>
@@ -2182,20 +2245,20 @@
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
-      <c r="E68" s="5"/>
+      <c r="E68" s="10"/>
       <c r="F68" s="1">
         <v>2</v>
       </c>
-      <c r="G68" s="8">
+      <c r="G68" s="5">
         <v>2.6102708416499998</v>
       </c>
-      <c r="H68" s="8">
+      <c r="H68" s="5">
         <v>2.62322264787</v>
       </c>
-      <c r="I68" s="8">
+      <c r="I68" s="5">
         <v>98.808371172099996</v>
       </c>
-      <c r="J68" s="8">
+      <c r="J68" s="5">
         <v>99.238128248899997</v>
       </c>
       <c r="K68" s="1"/>
@@ -2206,22 +2269,22 @@
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
-      <c r="E69" s="4" t="s">
+      <c r="E69" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F69" s="1">
         <v>1</v>
       </c>
-      <c r="G69" s="8">
+      <c r="G69" s="5">
         <v>2.6129111709199999</v>
       </c>
-      <c r="H69" s="8">
+      <c r="H69" s="5">
         <v>2.6343432094799999</v>
       </c>
-      <c r="I69" s="8">
+      <c r="I69" s="5">
         <v>99.264999157000005</v>
       </c>
-      <c r="J69" s="8">
+      <c r="J69" s="5">
         <v>100.178377634</v>
       </c>
       <c r="K69" s="1"/>
@@ -2232,20 +2295,20 @@
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
-      <c r="E70" s="4"/>
+      <c r="E70" s="7"/>
       <c r="F70" s="1">
         <v>2</v>
       </c>
-      <c r="G70" s="8">
+      <c r="G70" s="5">
         <v>2.5534832933799998</v>
       </c>
-      <c r="H70" s="8">
+      <c r="H70" s="5">
         <v>2.6063036911199999</v>
       </c>
-      <c r="I70" s="8">
+      <c r="I70" s="5">
         <v>94.176786882100004</v>
       </c>
-      <c r="J70" s="8">
+      <c r="J70" s="5">
         <v>96.097156294200005</v>
       </c>
       <c r="K70" s="1"/>
@@ -2256,22 +2319,22 @@
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
-      <c r="E71" s="4" t="s">
-        <v>17</v>
+      <c r="E71" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="F71" s="1">
         <v>1</v>
       </c>
-      <c r="G71" s="8">
+      <c r="G71" s="5">
         <v>2.6151759667899999</v>
       </c>
-      <c r="H71" s="8">
+      <c r="H71" s="5">
         <v>2.6199364696999998</v>
       </c>
-      <c r="I71" s="8">
+      <c r="I71" s="5">
         <v>98.885630393300005</v>
       </c>
-      <c r="J71" s="8">
+      <c r="J71" s="5">
         <v>98.890911711900003</v>
       </c>
       <c r="K71" s="1"/>
@@ -2282,20 +2345,20 @@
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
-      <c r="E72" s="4"/>
+      <c r="E72" s="7"/>
       <c r="F72" s="1">
         <v>2</v>
       </c>
-      <c r="G72" s="8">
+      <c r="G72" s="5">
         <v>2.6214421289200001</v>
       </c>
-      <c r="H72" s="8">
+      <c r="H72" s="5">
         <v>2.6177355608499999</v>
       </c>
-      <c r="I72" s="8">
+      <c r="I72" s="5">
         <v>98.9595136051</v>
       </c>
-      <c r="J72" s="8">
+      <c r="J72" s="5">
         <v>98.989598060299997</v>
       </c>
       <c r="K72" s="1"/>
@@ -2314,46 +2377,50 @@
       <c r="D73" s="2">
         <v>1</v>
       </c>
-      <c r="E73" s="4" t="s">
+      <c r="E73" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F73" s="1">
         <v>1</v>
       </c>
-      <c r="G73" s="8">
+      <c r="G73" s="5">
         <v>6.73416341233</v>
       </c>
-      <c r="H73" s="8">
+      <c r="H73" s="5">
         <v>6.7352017493699998</v>
       </c>
-      <c r="I73" s="8">
+      <c r="I73" s="5">
         <v>153.05391928500001</v>
       </c>
-      <c r="J73" s="8">
+      <c r="J73" s="5">
         <v>154.79421773999999</v>
       </c>
-      <c r="K73" s="1"/>
-      <c r="L73" s="1"/>
+      <c r="K73">
+        <v>6.7487279999999998</v>
+      </c>
+      <c r="L73">
+        <v>8.5829850000000008</v>
+      </c>
     </row>
     <row r="74" spans="1:12" ht="17" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
-      <c r="E74" s="4"/>
+      <c r="E74" s="7"/>
       <c r="F74" s="1">
         <v>2</v>
       </c>
-      <c r="G74" s="8">
+      <c r="G74" s="5">
         <v>6.7085914434599996</v>
       </c>
-      <c r="H74" s="8">
+      <c r="H74" s="5">
         <v>6.7316915167799998</v>
       </c>
-      <c r="I74" s="8">
+      <c r="I74" s="5">
         <v>154.051176513</v>
       </c>
-      <c r="J74" s="8">
+      <c r="J74" s="5">
         <v>152.72078616100001</v>
       </c>
       <c r="K74" s="1"/>
@@ -2364,22 +2431,22 @@
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
-      <c r="E75" s="4" t="s">
+      <c r="E75" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F75" s="1">
         <v>1</v>
       </c>
-      <c r="G75" s="8">
+      <c r="G75" s="5">
         <v>3.3848860724600001</v>
       </c>
-      <c r="H75" s="8">
+      <c r="H75" s="5">
         <v>7.3091018171600002</v>
       </c>
-      <c r="I75" s="8">
+      <c r="I75" s="5">
         <v>72.952807727600003</v>
       </c>
-      <c r="J75" s="8">
+      <c r="J75" s="5">
         <v>160.07327621900001</v>
       </c>
       <c r="K75" s="1"/>
@@ -2390,20 +2457,20 @@
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
-      <c r="E76" s="4"/>
+      <c r="E76" s="7"/>
       <c r="F76" s="1">
         <v>2</v>
       </c>
-      <c r="G76" s="8">
+      <c r="G76" s="5">
         <v>3.3409925444200002</v>
       </c>
-      <c r="H76" s="8">
+      <c r="H76" s="5">
         <v>7.2994383483999998</v>
       </c>
-      <c r="I76" s="8">
+      <c r="I76" s="5">
         <v>71.718857088299998</v>
       </c>
-      <c r="J76" s="8">
+      <c r="J76" s="5">
         <v>158.57013535999999</v>
       </c>
       <c r="K76" s="1"/>
@@ -2414,22 +2481,22 @@
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
-      <c r="E77" s="5" t="s">
+      <c r="E77" s="10" t="s">
         <v>15</v>
       </c>
       <c r="F77" s="1">
         <v>1</v>
       </c>
-      <c r="G77" s="8">
+      <c r="G77" s="5">
         <v>6.7654412423599997</v>
       </c>
-      <c r="H77" s="8">
+      <c r="H77" s="5">
         <v>6.7649059669099998</v>
       </c>
-      <c r="I77" s="8">
+      <c r="I77" s="5">
         <v>156.58079394500001</v>
       </c>
-      <c r="J77" s="8">
+      <c r="J77" s="5">
         <v>158.32858682099999</v>
       </c>
       <c r="K77" s="1"/>
@@ -2440,20 +2507,20 @@
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
-      <c r="E78" s="5"/>
+      <c r="E78" s="10"/>
       <c r="F78" s="1">
         <v>2</v>
       </c>
-      <c r="G78" s="8">
+      <c r="G78" s="5">
         <v>6.7334756229800004</v>
       </c>
-      <c r="H78" s="8">
+      <c r="H78" s="5">
         <v>6.7795997969000004</v>
       </c>
-      <c r="I78" s="8">
+      <c r="I78" s="5">
         <v>157.01637898600001</v>
       </c>
-      <c r="J78" s="8">
+      <c r="J78" s="5">
         <v>156.19809593799999</v>
       </c>
       <c r="K78" s="1"/>
@@ -2470,16 +2537,16 @@
       <c r="F79" s="1">
         <v>1</v>
       </c>
-      <c r="G79" s="8">
+      <c r="G79" s="5">
         <v>6.5275713300999998</v>
       </c>
-      <c r="H79" s="8">
+      <c r="H79" s="5">
         <v>6.7528548692200001</v>
       </c>
-      <c r="I79" s="8">
+      <c r="I79" s="5">
         <v>146.10985322799999</v>
       </c>
-      <c r="J79" s="8">
+      <c r="J79" s="5">
         <v>152.320125733</v>
       </c>
       <c r="K79" s="1"/>
@@ -2494,52 +2561,68 @@
       <c r="F80" s="1">
         <v>2</v>
       </c>
-      <c r="G80" s="8">
+      <c r="G80" s="5">
         <v>6.4779837218800003</v>
       </c>
-      <c r="H80" s="8">
+      <c r="H80" s="5">
         <v>6.8210908635200003</v>
       </c>
-      <c r="I80" s="8">
+      <c r="I80" s="5">
         <v>144.99233927700001</v>
       </c>
-      <c r="J80" s="8">
+      <c r="J80" s="5">
         <v>151.416139929</v>
       </c>
       <c r="K80" s="1"/>
       <c r="L80" s="1"/>
     </row>
-    <row r="81" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
-      <c r="E81" s="4" t="s">
-        <v>17</v>
+      <c r="E81" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="F81" s="1">
         <v>1</v>
       </c>
-      <c r="G81" s="9"/>
-      <c r="H81" s="9"/>
-      <c r="I81" s="9"/>
-      <c r="J81" s="9"/>
+      <c r="G81" s="5">
+        <v>6.7146351968899998</v>
+      </c>
+      <c r="H81" s="5">
+        <v>6.7352658410700004</v>
+      </c>
+      <c r="I81" s="5">
+        <v>152.63529995100001</v>
+      </c>
+      <c r="J81" s="5">
+        <v>155.060039636</v>
+      </c>
       <c r="K81" s="1"/>
       <c r="L81" s="1"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" ht="17" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
-      <c r="E82" s="4"/>
+      <c r="E82" s="7"/>
       <c r="F82" s="1">
         <v>2</v>
       </c>
-      <c r="G82" s="9"/>
-      <c r="H82" s="9"/>
-      <c r="I82" s="9"/>
-      <c r="J82" s="9"/>
+      <c r="G82" s="5">
+        <v>6.7302468391200003</v>
+      </c>
+      <c r="H82" s="5">
+        <v>6.7245562525600002</v>
+      </c>
+      <c r="I82" s="5">
+        <v>154.60700574699999</v>
+      </c>
+      <c r="J82" s="5">
+        <v>152.43307499900001</v>
+      </c>
       <c r="K82" s="1"/>
       <c r="L82" s="1"/>
     </row>
@@ -2556,46 +2639,50 @@
       <c r="D83" s="2">
         <v>3</v>
       </c>
-      <c r="E83" s="4" t="s">
+      <c r="E83" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F83" s="1">
         <v>1</v>
       </c>
-      <c r="G83" s="8">
+      <c r="G83" s="5">
         <v>3.28522056073</v>
       </c>
-      <c r="H83" s="8">
+      <c r="H83" s="5">
         <v>3.2836901490899999</v>
       </c>
-      <c r="I83" s="8">
+      <c r="I83" s="5">
         <v>109.630326372</v>
       </c>
-      <c r="J83" s="8">
+      <c r="J83" s="5">
         <v>109.850182934</v>
       </c>
-      <c r="K83" s="1"/>
-      <c r="L83" s="1"/>
+      <c r="K83">
+        <v>3.2757010000000002</v>
+      </c>
+      <c r="L83">
+        <v>4.2543540000000002</v>
+      </c>
     </row>
     <row r="84" spans="1:12" ht="17" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
-      <c r="E84" s="4"/>
+      <c r="E84" s="7"/>
       <c r="F84" s="1">
         <v>2</v>
       </c>
-      <c r="G84" s="8">
+      <c r="G84" s="5">
         <v>3.2824415275400001</v>
       </c>
-      <c r="H84" s="8">
+      <c r="H84" s="5">
         <v>3.2851110921700002</v>
       </c>
-      <c r="I84" s="8">
+      <c r="I84" s="5">
         <v>109.776033166</v>
       </c>
-      <c r="J84" s="8">
+      <c r="J84" s="5">
         <v>109.607125584</v>
       </c>
       <c r="K84" s="1"/>
@@ -2606,22 +2693,22 @@
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
-      <c r="E85" s="4" t="s">
+      <c r="E85" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F85" s="1">
         <v>1</v>
       </c>
-      <c r="G85" s="8">
+      <c r="G85" s="5">
         <v>2.35952368877</v>
       </c>
-      <c r="H85" s="8">
+      <c r="H85" s="5">
         <v>3.6848732273699998</v>
       </c>
-      <c r="I85" s="8">
+      <c r="I85" s="5">
         <v>72.651001462599993</v>
       </c>
-      <c r="J85" s="8">
+      <c r="J85" s="5">
         <v>115.37451654</v>
       </c>
       <c r="K85" s="1"/>
@@ -2632,20 +2719,20 @@
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
-      <c r="E86" s="4"/>
+      <c r="E86" s="7"/>
       <c r="F86" s="1">
         <v>2</v>
       </c>
-      <c r="G86" s="8">
+      <c r="G86" s="5">
         <v>2.3602039618299999</v>
       </c>
-      <c r="H86" s="8">
+      <c r="H86" s="5">
         <v>3.6919710930099998</v>
       </c>
-      <c r="I86" s="8">
+      <c r="I86" s="5">
         <v>73.012821556800006</v>
       </c>
-      <c r="J86" s="8">
+      <c r="J86" s="5">
         <v>115.621063992</v>
       </c>
       <c r="K86" s="1"/>
@@ -2656,22 +2743,22 @@
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
-      <c r="E87" s="5" t="s">
+      <c r="E87" s="10" t="s">
         <v>15</v>
       </c>
       <c r="F87" s="1">
         <v>1</v>
       </c>
-      <c r="G87" s="8">
+      <c r="G87" s="5">
         <v>3.28104476633</v>
       </c>
-      <c r="H87" s="8">
+      <c r="H87" s="5">
         <v>3.2827634469600002</v>
       </c>
-      <c r="I87" s="8">
+      <c r="I87" s="5">
         <v>109.61261058300001</v>
       </c>
-      <c r="J87" s="8">
+      <c r="J87" s="5">
         <v>109.954601594</v>
       </c>
       <c r="K87" s="1"/>
@@ -2682,20 +2769,20 @@
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
-      <c r="E88" s="5"/>
+      <c r="E88" s="10"/>
       <c r="F88" s="1">
         <v>2</v>
       </c>
-      <c r="G88" s="8">
+      <c r="G88" s="5">
         <v>3.2780105011499998</v>
       </c>
-      <c r="H88" s="8">
+      <c r="H88" s="5">
         <v>3.2861901473900001</v>
       </c>
-      <c r="I88" s="8">
+      <c r="I88" s="5">
         <v>109.752268653</v>
       </c>
-      <c r="J88" s="8">
+      <c r="J88" s="5">
         <v>109.734370524</v>
       </c>
       <c r="K88" s="1"/>
@@ -2712,20 +2799,18 @@
       <c r="F89" s="1">
         <v>1</v>
       </c>
-      <c r="G89" s="8">
+      <c r="G89" s="5">
         <v>3.2385138585200002</v>
       </c>
-      <c r="H89" s="8">
+      <c r="H89" s="5">
         <v>3.2771756987899998</v>
       </c>
-      <c r="I89" s="8">
+      <c r="I89" s="5">
         <v>105.969919064</v>
       </c>
-      <c r="J89" s="8">
+      <c r="J89" s="5">
         <v>107.54862799599999</v>
       </c>
-      <c r="K89" s="1"/>
-      <c r="L89" s="1"/>
     </row>
     <row r="90" spans="1:12" ht="17" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
@@ -2736,52 +2821,68 @@
       <c r="F90" s="1">
         <v>2</v>
       </c>
-      <c r="G90" s="8">
+      <c r="G90" s="5">
         <v>3.2163792331700001</v>
       </c>
-      <c r="H90" s="8">
+      <c r="H90" s="5">
         <v>3.2584776233300001</v>
       </c>
-      <c r="I90" s="8">
+      <c r="I90" s="5">
         <v>104.808656098</v>
       </c>
-      <c r="J90" s="8">
+      <c r="J90" s="5">
         <v>106.060457008</v>
       </c>
       <c r="K90" s="1"/>
       <c r="L90" s="1"/>
     </row>
-    <row r="91" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
-      <c r="E91" s="4" t="s">
-        <v>17</v>
+      <c r="E91" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="F91" s="1">
         <v>1</v>
       </c>
-      <c r="G91" s="9"/>
-      <c r="H91" s="9"/>
-      <c r="I91" s="9"/>
-      <c r="J91" s="9"/>
+      <c r="G91" s="5">
+        <v>3.2773451317000002</v>
+      </c>
+      <c r="H91" s="5">
+        <v>3.2843203077199998</v>
+      </c>
+      <c r="I91" s="5">
+        <v>109.72260210899999</v>
+      </c>
+      <c r="J91" s="5">
+        <v>108.914027143</v>
+      </c>
       <c r="K91" s="1"/>
       <c r="L91" s="1"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12" ht="17" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
-      <c r="E92" s="4"/>
+      <c r="E92" s="7"/>
       <c r="F92" s="1">
         <v>2</v>
       </c>
-      <c r="G92" s="9"/>
-      <c r="H92" s="9"/>
-      <c r="I92" s="9"/>
-      <c r="J92" s="9"/>
+      <c r="G92" s="5">
+        <v>3.2904286327099999</v>
+      </c>
+      <c r="H92" s="5">
+        <v>3.2846146512200001</v>
+      </c>
+      <c r="I92" s="5">
+        <v>109.69343657</v>
+      </c>
+      <c r="J92" s="5">
+        <v>110.53877333200001</v>
+      </c>
       <c r="K92" s="1"/>
       <c r="L92" s="1"/>
     </row>
@@ -2804,16 +2905,16 @@
       <c r="F93" s="1">
         <v>1</v>
       </c>
-      <c r="G93" s="8">
+      <c r="G93" s="5">
         <v>4.8145806048799997</v>
       </c>
-      <c r="H93" s="8">
+      <c r="H93" s="5">
         <v>4.8250475543600002</v>
       </c>
-      <c r="I93" s="8">
+      <c r="I93" s="5">
         <v>132.06304469099999</v>
       </c>
-      <c r="J93" s="8">
+      <c r="J93" s="5">
         <v>132.02729994000001</v>
       </c>
       <c r="K93">
@@ -2832,19 +2933,19 @@
       <c r="F94" s="1">
         <v>2</v>
       </c>
-      <c r="G94" s="8">
+      <c r="G94" s="5">
         <v>4.8266896942799997</v>
       </c>
-      <c r="H94" s="8">
+      <c r="H94" s="5">
         <v>4.8215483879400001</v>
       </c>
-      <c r="I94" s="8">
+      <c r="I94" s="5">
         <v>132.28401112200001</v>
       </c>
-      <c r="J94" s="8">
+      <c r="J94" s="5">
         <v>132.46461061599999</v>
       </c>
-      <c r="K94" s="9"/>
+      <c r="K94" s="6"/>
       <c r="L94" s="1"/>
     </row>
     <row r="95" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.25">
@@ -2852,22 +2953,22 @@
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
-      <c r="E95" s="4" t="s">
+      <c r="E95" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F95" s="1">
         <v>1</v>
       </c>
-      <c r="G95" s="8">
+      <c r="G95" s="5">
         <v>3.2367545607600001</v>
       </c>
-      <c r="H95" s="8">
+      <c r="H95" s="5">
         <v>5.47989047031</v>
       </c>
-      <c r="I95" s="8">
+      <c r="I95" s="5">
         <v>81.250578675599996</v>
       </c>
-      <c r="J95" s="8">
+      <c r="J95" s="5">
         <v>139.89130844799999</v>
       </c>
       <c r="K95" s="1"/>
@@ -2878,20 +2979,20 @@
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
-      <c r="E96" s="4"/>
+      <c r="E96" s="7"/>
       <c r="F96" s="1">
         <v>2</v>
       </c>
-      <c r="G96" s="8">
+      <c r="G96" s="5">
         <v>3.2539753688699999</v>
       </c>
-      <c r="H96" s="8">
+      <c r="H96" s="5">
         <v>5.47253899723</v>
       </c>
-      <c r="I96" s="8">
+      <c r="I96" s="5">
         <v>81.719057752599994</v>
       </c>
-      <c r="J96" s="8">
+      <c r="J96" s="5">
         <v>140.18479002000001</v>
       </c>
       <c r="K96" s="1"/>
@@ -2902,22 +3003,22 @@
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
-      <c r="E97" s="5" t="s">
+      <c r="E97" s="10" t="s">
         <v>15</v>
       </c>
       <c r="F97" s="1">
         <v>1</v>
       </c>
-      <c r="G97" s="8">
+      <c r="G97" s="5">
         <v>4.8062160688000004</v>
       </c>
-      <c r="H97" s="8">
+      <c r="H97" s="5">
         <v>4.8220398776</v>
       </c>
-      <c r="I97" s="8">
+      <c r="I97" s="5">
         <v>131.98481996999999</v>
       </c>
-      <c r="J97" s="8">
+      <c r="J97" s="5">
         <v>132.08472081900001</v>
       </c>
       <c r="K97" s="1"/>
@@ -2928,20 +3029,20 @@
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
-      <c r="E98" s="5"/>
+      <c r="E98" s="10"/>
       <c r="F98" s="1">
         <v>2</v>
       </c>
-      <c r="G98" s="8">
+      <c r="G98" s="5">
         <v>4.8187261472999996</v>
       </c>
-      <c r="H98" s="8">
+      <c r="H98" s="5">
         <v>0.82244493721</v>
       </c>
-      <c r="I98" s="8">
+      <c r="I98" s="5">
         <v>132.182824716</v>
       </c>
-      <c r="J98" s="8">
+      <c r="J98" s="5">
         <v>132.548714598</v>
       </c>
       <c r="K98" s="1"/>
@@ -2952,22 +3053,22 @@
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
-      <c r="E99" s="4" t="s">
+      <c r="E99" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F99" s="1">
         <v>1</v>
       </c>
-      <c r="G99" s="8">
+      <c r="G99" s="5">
         <v>4.7504728334899999</v>
       </c>
-      <c r="H99" s="8">
+      <c r="H99" s="5">
         <v>4.8367115524099997</v>
       </c>
-      <c r="I99" s="8">
+      <c r="I99" s="5">
         <v>128.98566759100001</v>
       </c>
-      <c r="J99" s="8">
+      <c r="J99" s="5">
         <v>131.15154848099999</v>
       </c>
       <c r="K99" s="1"/>
@@ -2978,20 +3079,20 @@
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
-      <c r="E100" s="4"/>
+      <c r="E100" s="7"/>
       <c r="F100" s="1">
         <v>2</v>
       </c>
-      <c r="G100" s="8">
+      <c r="G100" s="5">
         <v>4.8002579734599999</v>
       </c>
-      <c r="H100" s="8">
+      <c r="H100" s="5">
         <v>4.8987198762200004</v>
       </c>
-      <c r="I100" s="8">
+      <c r="I100" s="5">
         <v>131.71075893</v>
       </c>
-      <c r="J100" s="8">
+      <c r="J100" s="5">
         <v>134.68569237899999</v>
       </c>
       <c r="K100" s="1"/>
@@ -3002,22 +3103,22 @@
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
-      <c r="E101" s="4" t="s">
-        <v>17</v>
+      <c r="E101" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="F101" s="1">
         <v>1</v>
       </c>
-      <c r="G101" s="8">
+      <c r="G101" s="5">
         <v>4.8185731152600004</v>
       </c>
-      <c r="H101" s="8">
+      <c r="H101" s="5">
         <v>4.82595388927</v>
       </c>
-      <c r="I101" s="8">
+      <c r="I101" s="5">
         <v>131.77926890699999</v>
       </c>
-      <c r="J101" s="8">
+      <c r="J101" s="5">
         <v>132.99611972100001</v>
       </c>
       <c r="K101" s="1"/>
@@ -3028,20 +3129,20 @@
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
-      <c r="E102" s="4"/>
+      <c r="E102" s="7"/>
       <c r="F102" s="1">
         <v>2</v>
       </c>
-      <c r="G102" s="8">
+      <c r="G102" s="5">
         <v>4.8233727856900002</v>
       </c>
-      <c r="H102" s="8">
+      <c r="H102" s="5">
         <v>4.8189934548800002</v>
       </c>
-      <c r="I102" s="8">
+      <c r="I102" s="5">
         <v>132.57011378000001</v>
       </c>
-      <c r="J102" s="8">
+      <c r="J102" s="5">
         <v>131.482615049</v>
       </c>
       <c r="K102" s="1"/>

</xml_diff>